<commit_message>
Updated datasets after pre-processing
</commit_message>
<xml_diff>
--- a/data/interim_data/IPLBowlStatscleandata.xlsx
+++ b/data/interim_data/IPLBowlStatscleandata.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22666beef4f99752/Documents/Data Science/Springboard/SpringboardCapstone2/data/interim_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_23F921ED66C34B675F64403431436E064791D048" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC398DAB-2F50-4C96-9009-C7C63F0D854F}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -559,11 +565,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,6 +633,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -673,7 +687,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -705,9 +719,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -739,6 +771,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -914,14 +964,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="27.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -956,7 +1009,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -988,13 +1041,13 @@
         <v>23.82</v>
       </c>
       <c r="K2">
-        <v>8.380000000000001</v>
+        <v>8.3800000000000008</v>
       </c>
       <c r="L2">
         <v>17.05</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1032,7 +1085,7 @@
         <v>16.63</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1070,7 +1123,7 @@
         <v>19.55</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1108,7 +1161,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1146,7 +1199,7 @@
         <v>20.85</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1184,7 +1237,7 @@
         <v>24.84</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1222,7 +1275,7 @@
         <v>21.18</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1260,7 +1313,7 @@
         <v>22.75</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1298,7 +1351,7 @@
         <v>22.77</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1336,7 +1389,7 @@
         <v>18.91</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1374,7 +1427,7 @@
         <v>20.81</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1412,7 +1465,7 @@
         <v>24.28</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1447,10 +1500,10 @@
         <v>7.77</v>
       </c>
       <c r="L14">
-        <v>20.33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>20.329999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1485,10 +1538,10 @@
         <v>6.38</v>
       </c>
       <c r="L15">
-        <v>19.6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1520,13 +1573,13 @@
         <v>28.25</v>
       </c>
       <c r="K16">
-        <v>8.390000000000001</v>
+        <v>8.39</v>
       </c>
       <c r="L16">
         <v>20.2</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1564,7 +1617,7 @@
         <v>21.57</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1602,7 +1655,7 @@
         <v>25.28</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1640,7 +1693,7 @@
         <v>20.57</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1678,7 +1731,7 @@
         <v>14.42</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1716,7 +1769,7 @@
         <v>22.43</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1754,7 +1807,7 @@
         <v>16.34</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1792,7 +1845,7 @@
         <v>18.11</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1824,13 +1877,13 @@
         <v>26.85</v>
       </c>
       <c r="K24">
-        <v>8.449999999999999</v>
+        <v>8.4499999999999993</v>
       </c>
       <c r="L24">
         <v>19.07</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1868,7 +1921,7 @@
         <v>22.05</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1900,13 +1953,13 @@
         <v>26.9</v>
       </c>
       <c r="K26">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="L26">
         <v>19.45</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1938,13 +1991,13 @@
         <v>30.53</v>
       </c>
       <c r="K27">
-        <v>8.789999999999999</v>
+        <v>8.7899999999999991</v>
       </c>
       <c r="L27">
         <v>20.84</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1982,7 +2035,7 @@
         <v>19.72</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2011,7 +2064,7 @@
         <v>43160</v>
       </c>
       <c r="J29">
-        <v>36.12</v>
+        <v>36.119999999999997</v>
       </c>
       <c r="K29">
         <v>7.73</v>
@@ -2020,7 +2073,7 @@
         <v>28.04</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2052,13 +2105,13 @@
         <v>24.48</v>
       </c>
       <c r="K30">
-        <v>9.140000000000001</v>
+        <v>9.14</v>
       </c>
       <c r="L30">
         <v>16.07</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2090,13 +2143,13 @@
         <v>24.7</v>
       </c>
       <c r="K31">
-        <v>8.050000000000001</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="L31">
         <v>18.41</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2134,7 +2187,7 @@
         <v>20.78</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2166,13 +2219,13 @@
         <v>27.71</v>
       </c>
       <c r="K33">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="L33">
         <v>20.27</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2210,7 +2263,7 @@
         <v>19.09</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2248,7 +2301,7 @@
         <v>26.92</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2286,7 +2339,7 @@
         <v>16.05</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2321,10 +2374,10 @@
         <v>9.06</v>
       </c>
       <c r="L37">
-        <v>18.9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2362,7 +2415,7 @@
         <v>25.54</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2400,7 +2453,7 @@
         <v>21.16</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2432,13 +2485,13 @@
         <v>26.68</v>
       </c>
       <c r="K40">
-        <v>8.050000000000001</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="L40">
         <v>19.88</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2473,10 +2526,10 @@
         <v>7.52</v>
       </c>
       <c r="L41">
-        <v>18.31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
+        <v>18.309999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2511,10 +2564,10 @@
         <v>8.49</v>
       </c>
       <c r="L42">
-        <v>17.94</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
+        <v>17.940000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2546,13 +2599,13 @@
         <v>31.59</v>
       </c>
       <c r="K43">
-        <v>8.789999999999999</v>
+        <v>8.7899999999999991</v>
       </c>
       <c r="L43">
         <v>21.57</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2590,7 +2643,7 @@
         <v>22.21</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2628,7 +2681,7 @@
         <v>23.17</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2666,7 +2719,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2704,7 +2757,7 @@
         <v>23.56</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2742,7 +2795,7 @@
         <v>24.19</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2774,13 +2827,13 @@
         <v>27.9</v>
       </c>
       <c r="K49">
-        <v>8.289999999999999</v>
+        <v>8.2899999999999991</v>
       </c>
       <c r="L49">
         <v>20.2</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2818,7 +2871,7 @@
         <v>24.69</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2856,7 +2909,7 @@
         <v>19.57</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2885,7 +2938,7 @@
         <v>41699</v>
       </c>
       <c r="J52">
-        <v>33.41</v>
+        <v>33.409999999999997</v>
       </c>
       <c r="K52">
         <v>7.31</v>
@@ -2894,7 +2947,7 @@
         <v>27.41</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2932,7 +2985,7 @@
         <v>22.44</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2970,7 +3023,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3008,7 +3061,7 @@
         <v>20.71</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3040,13 +3093,13 @@
         <v>33.07</v>
       </c>
       <c r="K56">
-        <v>8.779999999999999</v>
+        <v>8.7799999999999994</v>
       </c>
       <c r="L56">
         <v>22.61</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3078,13 +3131,13 @@
         <v>29.98</v>
       </c>
       <c r="K57">
-        <v>8.630000000000001</v>
+        <v>8.6300000000000008</v>
       </c>
       <c r="L57">
         <v>20.84</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3122,7 +3175,7 @@
         <v>20.95</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3160,7 +3213,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3198,7 +3251,7 @@
         <v>21.04</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3236,7 +3289,7 @@
         <v>23.37</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3268,13 +3321,13 @@
         <v>26.16</v>
       </c>
       <c r="K62">
-        <v>8.109999999999999</v>
+        <v>8.11</v>
       </c>
       <c r="L62">
         <v>19.37</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3312,7 +3365,7 @@
         <v>16.82</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3350,7 +3403,7 @@
         <v>29.48</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -3388,7 +3441,7 @@
         <v>16.21</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3423,10 +3476,10 @@
         <v>7.7</v>
       </c>
       <c r="L66">
-        <v>17.85</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12">
+        <v>17.850000000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3464,7 +3517,7 @@
         <v>23.09</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3502,7 +3555,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -3540,7 +3593,7 @@
         <v>17.93</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -3578,7 +3631,7 @@
         <v>22.83</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -3616,7 +3669,7 @@
         <v>21.44</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3651,10 +3704,10 @@
         <v>7.55</v>
       </c>
       <c r="L72">
-        <v>18.49</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12">
+        <v>18.489999999999998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -3686,13 +3739,13 @@
         <v>23.09</v>
       </c>
       <c r="K73">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="L73">
         <v>16.89</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3724,13 +3777,13 @@
         <v>36.96</v>
       </c>
       <c r="K74">
-        <v>8.529999999999999</v>
+        <v>8.5299999999999994</v>
       </c>
       <c r="L74">
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3762,13 +3815,13 @@
         <v>30.16</v>
       </c>
       <c r="K75">
-        <v>8.539999999999999</v>
+        <v>8.5399999999999991</v>
       </c>
       <c r="L75">
         <v>21.18</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -3797,7 +3850,7 @@
         <v>42430</v>
       </c>
       <c r="J76">
-        <v>33.66</v>
+        <v>33.659999999999997</v>
       </c>
       <c r="K76">
         <v>8.94</v>
@@ -3806,7 +3859,7 @@
         <v>22.59</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3844,7 +3897,7 @@
         <v>15.86</v>
       </c>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3882,7 +3935,7 @@
         <v>27.31</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3914,13 +3967,13 @@
         <v>30.69</v>
       </c>
       <c r="K79">
-        <v>8.140000000000001</v>
+        <v>8.14</v>
       </c>
       <c r="L79">
         <v>22.62</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -3958,7 +4011,7 @@
         <v>16.29</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -3996,7 +4049,7 @@
         <v>23.14</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -4034,7 +4087,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -4072,7 +4125,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="84" spans="1:12">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -4104,13 +4157,13 @@
         <v>29.85</v>
       </c>
       <c r="K84">
-        <v>8.140000000000001</v>
+        <v>8.14</v>
       </c>
       <c r="L84">
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:12">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -4148,7 +4201,7 @@
         <v>18.93</v>
       </c>
     </row>
-    <row r="86" spans="1:12">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -4183,10 +4236,10 @@
         <v>8.27</v>
       </c>
       <c r="L86">
-        <v>19.15</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12">
+        <v>19.149999999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -4224,7 +4277,7 @@
         <v>23.24</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -4262,7 +4315,7 @@
         <v>19.97</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -4291,7 +4344,7 @@
         <v>43160</v>
       </c>
       <c r="J89">
-        <v>32.63</v>
+        <v>32.630000000000003</v>
       </c>
       <c r="K89">
         <v>8.67</v>
@@ -4300,7 +4353,7 @@
         <v>22.58</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -4332,13 +4385,13 @@
         <v>34.78</v>
       </c>
       <c r="K90">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="L90">
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:12">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -4376,7 +4429,7 @@
         <v>15.57</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -4414,7 +4467,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="93" spans="1:12">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -4452,7 +4505,7 @@
         <v>24.14</v>
       </c>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -4490,7 +4543,7 @@
         <v>21.25</v>
       </c>
     </row>
-    <row r="95" spans="1:12">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -4528,7 +4581,7 @@
         <v>24.17</v>
       </c>
     </row>
-    <row r="96" spans="1:12">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -4566,7 +4619,7 @@
         <v>21.06</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -4601,10 +4654,10 @@
         <v>7.17</v>
       </c>
       <c r="L97">
-        <v>17.06</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12">
+        <v>17.059999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -4636,13 +4689,13 @@
         <v>30.82</v>
       </c>
       <c r="K98">
-        <v>9.609999999999999</v>
+        <v>9.61</v>
       </c>
       <c r="L98">
-        <v>19.24</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12">
+        <v>19.239999999999998</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -4680,7 +4733,7 @@
         <v>17.45</v>
       </c>
     </row>
-    <row r="100" spans="1:12">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -4709,7 +4762,7 @@
         <v>42430</v>
       </c>
       <c r="J100">
-        <v>33.52</v>
+        <v>33.520000000000003</v>
       </c>
       <c r="K100">
         <v>7.23</v>
@@ -4718,7 +4771,7 @@
         <v>27.82</v>
       </c>
     </row>
-    <row r="101" spans="1:12">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -4750,13 +4803,13 @@
         <v>31.09</v>
       </c>
       <c r="K101">
-        <v>9.210000000000001</v>
+        <v>9.2100000000000009</v>
       </c>
       <c r="L101">
         <v>20.25</v>
       </c>
     </row>
-    <row r="102" spans="1:12">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -4794,7 +4847,7 @@
         <v>17.16</v>
       </c>
     </row>
-    <row r="103" spans="1:12">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -4832,7 +4885,7 @@
         <v>25.94</v>
       </c>
     </row>
-    <row r="104" spans="1:12">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -4861,7 +4914,7 @@
         <v>43891</v>
       </c>
       <c r="J104">
-        <v>32.77</v>
+        <v>32.770000000000003</v>
       </c>
       <c r="K104">
         <v>8.73</v>
@@ -4870,7 +4923,7 @@
         <v>22.52</v>
       </c>
     </row>
-    <row r="105" spans="1:12">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -4908,7 +4961,7 @@
         <v>37.06</v>
       </c>
     </row>
-    <row r="106" spans="1:12">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -4940,13 +4993,13 @@
         <v>21.93</v>
       </c>
       <c r="K106">
-        <v>8.970000000000001</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="L106">
         <v>14.67</v>
       </c>
     </row>
-    <row r="107" spans="1:12">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -4978,13 +5031,13 @@
         <v>31.4</v>
       </c>
       <c r="K107">
-        <v>8.710000000000001</v>
+        <v>8.7100000000000009</v>
       </c>
       <c r="L107">
         <v>21.63</v>
       </c>
     </row>
-    <row r="108" spans="1:12">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -5022,7 +5075,7 @@
         <v>26.97</v>
       </c>
     </row>
-    <row r="109" spans="1:12">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -5060,7 +5113,7 @@
         <v>18.52</v>
       </c>
     </row>
-    <row r="110" spans="1:12">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -5098,7 +5151,7 @@
         <v>23.57</v>
       </c>
     </row>
-    <row r="111" spans="1:12">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -5136,7 +5189,7 @@
         <v>16.89</v>
       </c>
     </row>
-    <row r="112" spans="1:12">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -5174,7 +5227,7 @@
         <v>24.39</v>
       </c>
     </row>
-    <row r="113" spans="1:12">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -5212,7 +5265,7 @@
         <v>28.07</v>
       </c>
     </row>
-    <row r="114" spans="1:12">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -5250,7 +5303,7 @@
         <v>29.3</v>
       </c>
     </row>
-    <row r="115" spans="1:12">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -5285,10 +5338,10 @@
         <v>9.32</v>
       </c>
       <c r="L115">
-        <v>19.85</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12">
+        <v>19.850000000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -5326,7 +5379,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -5364,7 +5417,7 @@
         <v>20.73</v>
       </c>
     </row>
-    <row r="118" spans="1:12">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -5393,7 +5446,7 @@
         <v>43221</v>
       </c>
       <c r="J118">
-        <v>18.85</v>
+        <v>18.850000000000001</v>
       </c>
       <c r="K118">
         <v>7.78</v>
@@ -5402,7 +5455,7 @@
         <v>14.54</v>
       </c>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -5431,16 +5484,16 @@
         <v>45203</v>
       </c>
       <c r="J119">
-        <v>17.92</v>
+        <v>17.920000000000002</v>
       </c>
       <c r="K119">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="L119">
         <v>12.96</v>
       </c>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -5478,7 +5531,7 @@
         <v>27.76</v>
       </c>
     </row>
-    <row r="121" spans="1:12">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -5516,7 +5569,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="122" spans="1:12">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -5554,7 +5607,7 @@
         <v>20.28</v>
       </c>
     </row>
-    <row r="123" spans="1:12">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -5592,7 +5645,7 @@
         <v>36.32</v>
       </c>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -5630,7 +5683,7 @@
         <v>22.04</v>
       </c>
     </row>
-    <row r="125" spans="1:12">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -5668,7 +5721,7 @@
         <v>23.08</v>
       </c>
     </row>
-    <row r="126" spans="1:12">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -5706,7 +5759,7 @@
         <v>15.29</v>
       </c>
     </row>
-    <row r="127" spans="1:12">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -5744,7 +5797,7 @@
         <v>16.29</v>
       </c>
     </row>
-    <row r="128" spans="1:12">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -5782,7 +5835,7 @@
         <v>25.08</v>
       </c>
     </row>
-    <row r="129" spans="1:12">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -5820,7 +5873,7 @@
         <v>19.91</v>
       </c>
     </row>
-    <row r="130" spans="1:12">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -5852,13 +5905,13 @@
         <v>27.83</v>
       </c>
       <c r="K130">
-        <v>8.119999999999999</v>
+        <v>8.1199999999999992</v>
       </c>
       <c r="L130">
         <v>20.57</v>
       </c>
     </row>
-    <row r="131" spans="1:12">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -5896,7 +5949,7 @@
         <v>15.65</v>
       </c>
     </row>
-    <row r="132" spans="1:12">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -5934,7 +5987,7 @@
         <v>29.48</v>
       </c>
     </row>
-    <row r="133" spans="1:12">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -5972,7 +6025,7 @@
         <v>16.91</v>
       </c>
     </row>
-    <row r="134" spans="1:12">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -6001,7 +6054,7 @@
         <v>41671</v>
       </c>
       <c r="J134">
-        <v>34.45</v>
+        <v>34.450000000000003</v>
       </c>
       <c r="K134">
         <v>7.66</v>
@@ -6010,7 +6063,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="135" spans="1:12">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -6039,7 +6092,7 @@
         <v>47178</v>
       </c>
       <c r="J135">
-        <v>38.45</v>
+        <v>38.450000000000003</v>
       </c>
       <c r="K135">
         <v>9.74</v>
@@ -6048,7 +6101,7 @@
         <v>23.68</v>
       </c>
     </row>
-    <row r="136" spans="1:12">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -6086,7 +6139,7 @@
         <v>30.38</v>
       </c>
     </row>
-    <row r="137" spans="1:12">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -6124,7 +6177,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="138" spans="1:12">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -6156,13 +6209,13 @@
         <v>23.7</v>
       </c>
       <c r="K138">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="L138">
-        <v>16.35</v>
-      </c>
-    </row>
-    <row r="139" spans="1:12">
+        <v>16.350000000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -6191,7 +6244,7 @@
         <v>44256</v>
       </c>
       <c r="J139">
-        <v>33.7</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="K139">
         <v>7.67</v>
@@ -6200,7 +6253,7 @@
         <v>26.35</v>
       </c>
     </row>
-    <row r="140" spans="1:12">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -6238,7 +6291,7 @@
         <v>31.1</v>
       </c>
     </row>
-    <row r="141" spans="1:12">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -6270,13 +6323,13 @@
         <v>24.84</v>
       </c>
       <c r="K141">
-        <v>8.449999999999999</v>
+        <v>8.4499999999999993</v>
       </c>
       <c r="L141">
         <v>17.63</v>
       </c>
     </row>
-    <row r="142" spans="1:12">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -6314,7 +6367,7 @@
         <v>22.84</v>
       </c>
     </row>
-    <row r="143" spans="1:12">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -6343,7 +6396,7 @@
         <v>45778</v>
       </c>
       <c r="J143">
-        <v>18.74</v>
+        <v>18.739999999999998</v>
       </c>
       <c r="K143">
         <v>6.94</v>
@@ -6352,7 +6405,7 @@
         <v>16.21</v>
       </c>
     </row>
-    <row r="144" spans="1:12">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -6390,7 +6443,7 @@
         <v>22.11</v>
       </c>
     </row>
-    <row r="145" spans="1:12">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -6428,7 +6481,7 @@
         <v>25.67</v>
       </c>
     </row>
-    <row r="146" spans="1:12">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -6466,7 +6519,7 @@
         <v>26.83</v>
       </c>
     </row>
-    <row r="147" spans="1:12">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -6504,7 +6557,7 @@
         <v>30.78</v>
       </c>
     </row>
-    <row r="148" spans="1:12">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -6542,7 +6595,7 @@
         <v>22.89</v>
       </c>
     </row>
-    <row r="149" spans="1:12">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -6580,7 +6633,7 @@
         <v>26.67</v>
       </c>
     </row>
-    <row r="150" spans="1:12">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -6618,7 +6671,7 @@
         <v>25.06</v>
       </c>
     </row>
-    <row r="151" spans="1:12">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -6656,7 +6709,7 @@
         <v>21.18</v>
       </c>
     </row>
-    <row r="152" spans="1:12">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -6694,7 +6747,7 @@
         <v>22.24</v>
       </c>
     </row>
-    <row r="153" spans="1:12">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -6732,7 +6785,7 @@
         <v>22.6</v>
       </c>
     </row>
-    <row r="154" spans="1:12">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -6764,13 +6817,13 @@
         <v>29.8</v>
       </c>
       <c r="K154">
-        <v>8.539999999999999</v>
+        <v>8.5399999999999991</v>
       </c>
       <c r="L154">
         <v>20.93</v>
       </c>
     </row>
-    <row r="155" spans="1:12">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -6808,7 +6861,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="156" spans="1:12">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -6840,13 +6893,13 @@
         <v>39.14</v>
       </c>
       <c r="K156">
-        <v>9.130000000000001</v>
+        <v>9.1300000000000008</v>
       </c>
       <c r="L156">
         <v>25.71</v>
       </c>
     </row>
-    <row r="157" spans="1:12">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -6878,13 +6931,13 @@
         <v>37.36</v>
       </c>
       <c r="K157">
-        <v>8.720000000000001</v>
+        <v>8.7200000000000006</v>
       </c>
       <c r="L157">
         <v>25.71</v>
       </c>
     </row>
-    <row r="158" spans="1:12">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -6916,13 +6969,13 @@
         <v>40.71</v>
       </c>
       <c r="K158">
-        <v>9.470000000000001</v>
+        <v>9.4700000000000006</v>
       </c>
       <c r="L158">
         <v>25.79</v>
       </c>
     </row>
-    <row r="159" spans="1:12">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -6960,7 +7013,7 @@
         <v>26.38</v>
       </c>
     </row>
-    <row r="160" spans="1:12">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -6998,7 +7051,7 @@
         <v>26.85</v>
       </c>
     </row>
-    <row r="161" spans="1:12">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -7033,10 +7086,10 @@
         <v>7.42</v>
       </c>
       <c r="L161">
-        <v>32.77</v>
-      </c>
-    </row>
-    <row r="162" spans="1:12">
+        <v>32.770000000000003</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -7074,7 +7127,7 @@
         <v>25.38</v>
       </c>
     </row>
-    <row r="163" spans="1:12">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -7112,7 +7165,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="164" spans="1:12">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -7150,7 +7203,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="165" spans="1:12">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -7188,7 +7241,7 @@
         <v>30.58</v>
       </c>
     </row>
-    <row r="166" spans="1:12">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -7226,7 +7279,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="167" spans="1:12">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -7258,13 +7311,13 @@
         <v>50.1</v>
       </c>
       <c r="K167">
-        <v>8.609999999999999</v>
+        <v>8.61</v>
       </c>
       <c r="L167">
         <v>34.9</v>
       </c>
     </row>
-    <row r="168" spans="1:12">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -7302,7 +7355,7 @@
         <v>45.75</v>
       </c>
     </row>
-    <row r="169" spans="1:12">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -7334,10 +7387,10 @@
         <v>59.25</v>
       </c>
       <c r="K169">
-        <v>8.970000000000001</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="L169">
-        <v>39.63</v>
+        <v>39.630000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>